<commit_message>
solved a bunch of minor bugs
</commit_message>
<xml_diff>
--- a/in/tri_Composant_Couleur.xlsx
+++ b/in/tri_Composant_Couleur.xlsx
@@ -5,24 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\Downloads\Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Extraction\MedievalAvignon\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B97F1-5BF3-4A66-BE28-C5B320459054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0E1F5-6BB1-4AF0-AF9A-0F193E48FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tri_Composant" sheetId="1" r:id="rId1"/>
-    <sheet name="typeComposant" sheetId="2" r:id="rId2"/>
-    <sheet name="typeSimpleComposant" sheetId="3" r:id="rId3"/>
+    <sheet name="mapComposantN" sheetId="1" r:id="rId1"/>
+    <sheet name="colorComposantN" sheetId="4" r:id="rId2"/>
+    <sheet name="typeComposant" sheetId="2" r:id="rId3"/>
+    <sheet name="typeSimpleComposant" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">colorComposantN!$A$1:$B$43</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="147">
   <si>
     <t>anniversaire</t>
   </si>
@@ -382,13 +396,94 @@
   </si>
   <si>
     <t>emplacement bat</t>
+  </si>
+  <si>
+    <t>#BF8100</t>
+  </si>
+  <si>
+    <t>#DCAA61</t>
+  </si>
+  <si>
+    <t>#C59956</t>
+  </si>
+  <si>
+    <t>#642D04</t>
+  </si>
+  <si>
+    <t>#944800</t>
+  </si>
+  <si>
+    <t>#FED200</t>
+  </si>
+  <si>
+    <t>#525252</t>
+  </si>
+  <si>
+    <t>#969696</t>
+  </si>
+  <si>
+    <t>#737373</t>
+  </si>
+  <si>
+    <t>#FFFFE9</t>
+  </si>
+  <si>
+    <t>#FFD966</t>
+  </si>
+  <si>
+    <t>#FFEB88</t>
+  </si>
+  <si>
+    <t>#FFB166</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>#BDBDBD</t>
+  </si>
+  <si>
+    <t>#41B6C4</t>
+  </si>
+  <si>
+    <t>#74C476</t>
+  </si>
+  <si>
+    <t>C09E70</t>
+  </si>
+  <si>
+    <t>#FEE8C8</t>
+  </si>
+  <si>
+    <t>#D9D9D9</t>
+  </si>
+  <si>
+    <t>#BF812D</t>
+  </si>
+  <si>
+    <t>#005A32</t>
+  </si>
+  <si>
+    <t>#41AB5D</t>
+  </si>
+  <si>
+    <t>#238B45</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Couleur</t>
+  </si>
+  <si>
+    <t>#C09E70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -523,8 +618,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="48">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,6 +892,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF7EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -955,7 +1062,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -974,6 +1081,9 @@
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1343,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1355,655 +1465,881 @@
     <col min="2" max="2" width="52.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C15" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>118</v>
+      </c>
+      <c r="C75" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2015,6 +2351,421 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0119B-750C-4933-9499-B9AD3FE27D1D}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -2157,7 +2908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
added comparison between estate and flat coms
</commit_message>
<xml_diff>
--- a/in/tri_Composant_Couleur.xlsx
+++ b/in/tri_Composant_Couleur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Extraction\MedievalAvignon\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0E1F5-6BB1-4AF0-AF9A-0F193E48FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB705F-0462-4A2C-8B7A-1963D9E047CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="typeSimpleComposant" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">colorComposantN!$A$1:$B$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">colorComposantN!$A$1:$B$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="149">
   <si>
     <t>anniversaire</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>#C09E70</t>
+  </si>
+  <si>
+    <t>#FFEDD4</t>
+  </si>
+  <si>
+    <t>trop clair (se confond avec le blanc)</t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -891,13 +897,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF7EC"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFEDD4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1062,7 +1074,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1079,11 +1091,12 @@
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1133,6 +1146,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFEDD4"/>
       <color rgb="FFFFB166"/>
       <color rgb="FFFFEB88"/>
       <color rgb="FFFFEBC8"/>
@@ -1142,7 +1156,6 @@
       <color rgb="FFFED099"/>
       <color rgb="FFFED02B"/>
       <color rgb="FFFFF8F0"/>
-      <color rgb="FF73EFE6"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1455,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1659,10 +1672,10 @@
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="17"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1693,7 +1706,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2352,10 +2365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0119B-750C-4933-9499-B9AD3FE27D1D}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2364,10 +2377,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2512,10 +2525,10 @@
       <c r="A15" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="17"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2540,7 +2553,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2609,154 +2622,175 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="21"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="21"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>101</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2770,7 +2804,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2807,8 +2841,8 @@
       <c r="A4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>101</v>
+      <c r="B4" s="20" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2905,6 +2939,7 @@
     <sortCondition ref="A1:A15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solved a few minor bugs
</commit_message>
<xml_diff>
--- a/in/tri_Composant_Couleur.xlsx
+++ b/in/tri_Composant_Couleur.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Extraction\MedievalAvignon\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB705F-0462-4A2C-8B7A-1963D9E047CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CFE206-A567-4EDE-88E9-84A6DFB08BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mapComposantN" sheetId="1" r:id="rId1"/>
-    <sheet name="colorComposantN" sheetId="4" r:id="rId2"/>
-    <sheet name="typeComposant" sheetId="2" r:id="rId3"/>
-    <sheet name="typeSimpleComposant" sheetId="3" r:id="rId4"/>
+    <sheet name="ComposantN_map" sheetId="1" r:id="rId1"/>
+    <sheet name="ComposantN_clr" sheetId="4" r:id="rId2"/>
+    <sheet name="typeComposant_clr" sheetId="2" r:id="rId3"/>
+    <sheet name="typeSimpleComposant_clr" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">colorComposantN!$A$1:$B$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ComposantN_clr!$A$1:$B$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="153">
   <si>
     <t>anniversaire</t>
   </si>
@@ -437,9 +437,6 @@
     <t>#FFB166</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>#BDBDBD</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>#74C476</t>
   </si>
   <si>
-    <t>C09E70</t>
-  </si>
-  <si>
     <t>#FEE8C8</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>#238B45</t>
   </si>
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
     <t>Couleur</t>
   </si>
   <si>
@@ -482,14 +473,35 @@
     <t>#FFEDD4</t>
   </si>
   <si>
-    <t>trop clair (se confond avec le blanc)</t>
+    <t>#0D0D0D</t>
+  </si>
+  <si>
+    <t>#FEC0C8</t>
+  </si>
+  <si>
+    <t>#942193</t>
+  </si>
+  <si>
+    <t>#DAADCC</t>
+  </si>
+  <si>
+    <t>Componsant</t>
+  </si>
+  <si>
+    <t>Composant normalisé</t>
+  </si>
+  <si>
+    <t>Type de composant</t>
+  </si>
+  <si>
+    <t>Type de composant simplifié</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -630,8 +642,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFD4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="50">
+  <fills count="77">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,12 +928,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFF7EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF8100"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDBDBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCAA61"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC59956"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF41B6C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF642D04"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF944800"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF74C476"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC09E70"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFED200"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D0D0D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF525252"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF969696"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF737373"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE8C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEC0C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF941993"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF812D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF005A32"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB88"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB166"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF41AB5D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF238B45"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3ABCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1029,6 +1210,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1074,7 +1264,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1093,10 +1283,36 @@
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="62" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="65" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="67" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="68" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="69" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="70" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="71" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="73" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="74" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="75" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="76" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="47" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1466,898 +1682,679 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
-        <v>133</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>133</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>133</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>102</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C14" t="s">
-        <v>133</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>109</v>
+      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" t="s">
-        <v>135</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" t="s">
-        <v>93</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C20" t="s">
-        <v>133</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C38" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>47</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C50" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>50</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C52" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>53</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C56" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>55</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C58" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C59" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C60" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>59</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C64" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C65" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C66" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C67" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>66</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C69" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>68</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C71" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C72" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C74" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C75" t="s">
-        <v>133</v>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C75">
-    <sortCondition ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B76">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
@@ -2365,431 +2362,432 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0119B-750C-4933-9499-B9AD3FE27D1D}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>103</v>
       </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="20" t="s">
         <v>120</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>134</v>
-      </c>
+      <c r="B6" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="22" t="s">
         <v>121</v>
       </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>100</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="23" t="s">
         <v>122</v>
       </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>102</v>
       </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>97</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="14" t="s">
         <v>98</v>
       </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B13" t="s">
-        <v>135</v>
-      </c>
+      <c r="B13" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="25" t="s">
         <v>123</v>
       </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="26" t="s">
         <v>124</v>
       </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="14" t="s">
         <v>98</v>
       </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
-        <v>136</v>
-      </c>
+      <c r="B20" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="29" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="21"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="31" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="33" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="21"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B36" s="21"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="40" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="41" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="42" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B45" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B46" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="21" t="s">
+      <c r="B46" s="45" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2801,142 +2799,149 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="1"/>
+      <c r="A1" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>100</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>147</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>103</v>
+        <v>77</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>104</v>
+        <v>50</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>102</v>
+        <v>84</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>79</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>105</v>
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>99</v>
+        <v>82</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
-    <sortCondition ref="A1:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2945,58 +2950,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>89</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>90</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>